<commit_message>
got a moving sprite
</commit_message>
<xml_diff>
--- a/credits.xlsx
+++ b/credits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Gene-Hunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9487A-E30B-4698-9439-5993045F9137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52E680A-80DC-4630-99B7-7928685405CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1995" windowWidth="24780" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="1935" windowWidth="14145" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Snorri Sturluson</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>https://snorristurluson.github.io/CustomSlateWidgets/</t>
+  </si>
+  <si>
+    <t>Character base (dummy)</t>
+  </si>
+  <si>
+    <t>Bagong Games</t>
+  </si>
+  <si>
+    <t>https://bagong-games.itch.io/hana-caraka-base-character</t>
   </si>
 </sst>
 </file>
@@ -363,13 +372,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -394,6 +409,17 @@
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
realllly cooking with movement now!
</commit_message>
<xml_diff>
--- a/credits.xlsx
+++ b/credits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Gene-Hunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310E14E6-275F-4706-A72D-178E2CCEBFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E226C3-4FD5-442E-B458-FC1AA5490447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8160" yWindow="1935" windowWidth="14145" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Snorri Sturluson</t>
   </si>
@@ -48,9 +48,6 @@
     <t>https://snorristurluson.github.io/CustomSlateWidgets/</t>
   </si>
   <si>
-    <t>Probably not used in the final version</t>
-  </si>
-  <si>
     <t>PaperZD Tutorial</t>
   </si>
   <si>
@@ -60,13 +57,43 @@
     <t>https://www.youtube.com/watch?v=aWkgOr5U-zI</t>
   </si>
   <si>
-    <t>Placeholder sprite characters</t>
-  </si>
-  <si>
     <t>Craftpix.net</t>
   </si>
   <si>
     <t>https://free-game-assets.itch.io/free-tiny-hero-sprites-pixel-art</t>
+  </si>
+  <si>
+    <t>Dude Monster</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>Valla</t>
+  </si>
+  <si>
+    <t>Badim</t>
+  </si>
+  <si>
+    <t>https://badim.itch.io/pixelart-valla</t>
+  </si>
+  <si>
+    <t>Slimes</t>
+  </si>
+  <si>
+    <t>Shimmy</t>
+  </si>
+  <si>
+    <t>https://shimyx.itch.io/6-direction-slimes-animation</t>
+  </si>
+  <si>
+    <t>2D Topdown Tutorial</t>
+  </si>
+  <si>
+    <t>Cobra Code</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=z1RMDMKcROQ</t>
   </si>
 </sst>
 </file>
@@ -384,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,27 +452,66 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>